<commit_message>
Fix total error counting
Separate data for learning and testing.
</commit_message>
<xml_diff>
--- a/src/data05.xlsx
+++ b/src/data05.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
   <si>
     <t xml:space="preserve">0.842</t>
   </si>
@@ -470,99 +470,6 @@
   </si>
   <si>
     <t xml:space="preserve">0.925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.161</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.278</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.899</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.687</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.702</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.275</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.553</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.723</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.562</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.381</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.856</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.848</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.492</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.609</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.348</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.711</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.755</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.807</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.462</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.455</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.361</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.989</t>
   </si>
 </sst>
 </file>
@@ -577,6 +484,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -658,17 +566,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E88" activeCellId="0" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="6.01020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.53571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.80612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,237 +1446,6 @@
       </c>
       <c r="C79" s="0" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C80" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="C81" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C82" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="C83" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C84" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="C85" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="C86" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="C87" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C88" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B89" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="C89" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="B90" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C90" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B91" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C91" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="B92" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="C92" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B93" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="C93" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="B94" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="C94" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="B95" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C95" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="B96" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C96" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B97" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="C97" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B98" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="C98" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B99" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C99" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B100" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="C100" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>